<commit_message>
summary of the experiments
</commit_message>
<xml_diff>
--- a/Diabetes/Traditional vs 11 features for prof _V3/Book2-NoHBP.xlsx
+++ b/Diabetes/Traditional vs 11 features for prof _V3/Book2-NoHBP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkPlace\github projects\Health-Data-Analysis-Diabetics\Diabetes\Traditional vs 11 features for prof _V3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E979DD-F782-4E1B-9A9C-75169EA6C6B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86465E29-E3F6-43BA-8414-F94B37B2DD0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E74EC6CB-DB7C-45A2-A2A5-D2690C62073B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E74EC6CB-DB7C-45A2-A2A5-D2690C62073B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -10933,10 +10933,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10B1093B-955B-44EA-8DB3-C21F7774908B}">
-  <dimension ref="C5:N26"/>
+  <dimension ref="C5:N29"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AE13" sqref="AE13"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11487,6 +11487,18 @@
       </c>
     </row>
     <row r="26" spans="3:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="N28">
+        <f>MAX(N20:N25)</f>
+        <v>0.74970000000000003</v>
+      </c>
+    </row>
+    <row r="29" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <f>MAX(D20:M25)</f>
+        <v>0.753</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -11495,10 +11507,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90595FF6-D4F2-497D-8BE6-C59F0FCE2E87}">
-  <dimension ref="C5:K56"/>
+  <dimension ref="B5:K56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:K8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11507,7 +11519,7 @@
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D5">
         <v>5</v>
       </c>
@@ -11533,7 +11545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>2</v>
       </c>
@@ -11562,7 +11574,7 @@
         <v>0.73499999999999999</v>
       </c>
     </row>
-    <row r="7" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>3</v>
       </c>
@@ -11591,7 +11603,7 @@
         <v>0.72333333333333305</v>
       </c>
     </row>
-    <row r="8" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>4</v>
       </c>
@@ -11617,6 +11629,68 @@
         <v>0.74</v>
       </c>
       <c r="K8">
+        <v>0.72333333333333305</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <f>AVERAGE(D6:K8)</f>
+        <v>0.74170833333333297</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <f>AVERAGE(D6:D8)</f>
+        <v>0.74888888888888872</v>
+      </c>
+      <c r="E11">
+        <f t="shared" ref="E11:K11" si="0">AVERAGE(E6:E8)</f>
+        <v>0.74199999999999966</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>0.74666666666666626</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>0.74388888888888849</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>0.74444444444444435</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>0.74388888888888871</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>0.73666666666666669</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="0"/>
+        <v>0.7272222222222221</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <f>MAX(D6:K8)</f>
+        <v>0.75166666666666604</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <f>MIN(D6:K8)</f>
+        <v>0.72333333333333305</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>0.75166666666666604</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17">
         <v>0.72333333333333305</v>
       </c>
     </row>
@@ -11881,7 +11955,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{106AA715-0EBF-4614-813D-E0D496B8BE8F}">
   <dimension ref="D7:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U15" sqref="U15"/>
     </sheetView>
   </sheetViews>

</xml_diff>